<commit_message>
Se separa la logica del driver en un JAR
</commit_message>
<xml_diff>
--- a/src/test/resources/data.xlsx
+++ b/src/test/resources/data.xlsx
@@ -3,8 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="COMPROBANTES" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="KIASKDAISD" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="DUDA" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -12,34 +11,25 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>testCaseId</t>
+    <t>ID</t>
   </si>
   <si>
-    <t>hola</t>
+    <t>NombreEquipo</t>
   </si>
   <si>
-    <t>apellido</t>
+    <t>@11</t>
   </si>
   <si>
-    <t>@HB-8966</t>
-  </si>
-  <si>
-    <t>JUAN</t>
-  </si>
-  <si>
-    <t>BRITO</t>
-  </si>
-  <si>
-    <t>@HB-8967</t>
+    <t>Smart Tv</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+  <fonts count="2">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -47,70 +37,30 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <color rgb="FF000000"/>
-      <name val="Roboto"/>
-    </font>
-    <font>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <color rgb="FF000000"/>
-      <name val="&quot;JetBrains Mono&quot;"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF1E1F22"/>
-        <bgColor rgb="FF1E1F22"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border/>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -122,10 +72,6 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -332,49 +278,31 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="9.5"/>
+    <col customWidth="1" min="2" max="2" width="11.63"/>
+    <col customWidth="1" min="3" max="3" width="12.63"/>
+    <col customWidth="1" min="4" max="4" width="16.5"/>
+    <col customWidth="1" min="5" max="5" width="17.25"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="3" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
-  <sheetData/>
-  <drawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>